<commit_message>
updating the results and Origin file
</commit_message>
<xml_diff>
--- a/IEEETransactionOnIntelligent/scenarios.xlsb.xlsx
+++ b/IEEETransactionOnIntelligent/scenarios.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\matlab_workspace\SchedulingSimulation\IEEETransactionOnIntelligent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00BB0C2-4DCC-46F6-A51D-83C2CCBFE6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8979A7D-0028-400D-9B67-667F24DCF107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="16584" windowHeight="8808" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40770" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TrafficMetric" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Scenario1-revised" sheetId="5" r:id="rId3"/>
     <sheet name="Scenario2" sheetId="4" r:id="rId4"/>
     <sheet name="Scenario3" sheetId="6" r:id="rId5"/>
+    <sheet name="Scenario4" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="39">
   <si>
     <t>u_min</t>
   </si>
@@ -154,6 +155,9 @@
   </si>
   <si>
     <t>The seed number is for the random generator in Matlab</t>
+  </si>
+  <si>
+    <t>flow rate</t>
   </si>
 </sst>
 </file>
@@ -426,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -625,6 +629,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -938,10 +954,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="72"/>
+      <c r="M1" s="76"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
@@ -1190,23 +1206,23 @@
       <c r="M7">
         <v>2E-3</v>
       </c>
-      <c r="R7" s="72" t="s">
+      <c r="R7" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="72"/>
+      <c r="S7" s="76"/>
       <c r="T7" s="2"/>
-      <c r="U7" s="72" t="s">
+      <c r="U7" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="V7" s="72"/>
-      <c r="W7" s="72" t="s">
+      <c r="V7" s="76"/>
+      <c r="W7" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="X7" s="72"/>
-      <c r="Y7" s="72" t="s">
+      <c r="X7" s="76"/>
+      <c r="Y7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="Z7" s="72"/>
+      <c r="Z7" s="76"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1693,24 +1709,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72" t="s">
+      <c r="I3" s="76"/>
+      <c r="J3" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72" t="s">
+      <c r="K3" s="76"/>
+      <c r="L3" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="72"/>
+      <c r="M3" s="76"/>
       <c r="N3" t="s">
         <v>10</v>
       </c>
@@ -3139,24 +3155,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72" t="s">
+      <c r="I3" s="76"/>
+      <c r="J3" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72" t="s">
+      <c r="K3" s="76"/>
+      <c r="L3" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="72"/>
+      <c r="M3" s="76"/>
       <c r="N3" t="s">
         <v>10</v>
       </c>
@@ -4606,33 +4622,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73" t="s">
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
     </row>
     <row r="4" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
@@ -4667,16 +4683,16 @@
       </c>
       <c r="L4" s="32"/>
       <c r="M4" s="32"/>
-      <c r="N4" s="73" t="s">
+      <c r="N4" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73" t="s">
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
     </row>
     <row r="5" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="37">
@@ -6146,8 +6162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC876E74-9F2E-4384-8020-8E7038E88A03}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6173,33 +6189,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73" t="s">
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
     </row>
     <row r="4" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="70" t="s">
@@ -6234,28 +6250,42 @@
       </c>
       <c r="L4" s="69"/>
       <c r="M4" s="69"/>
-      <c r="N4" s="73" t="s">
+      <c r="N4" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73" t="s">
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
     </row>
     <row r="5" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="37">
         <v>8</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
+      <c r="D5" s="38">
+        <v>15</v>
+      </c>
+      <c r="E5" s="38">
+        <v>40.603999999999999</v>
+      </c>
+      <c r="F5" s="38">
+        <v>40.603999999999999</v>
+      </c>
+      <c r="G5" s="38">
+        <v>49.9587</v>
+      </c>
+      <c r="H5" s="38">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="I5" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="J5" s="39">
+        <v>1.7399999999999999E-2</v>
+      </c>
       <c r="L5" s="34" t="s">
         <v>23</v>
       </c>
@@ -6285,160 +6315,216 @@
       <c r="C6" s="40">
         <v>8</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="41"/>
+      <c r="D6" s="33">
+        <v>30</v>
+      </c>
+      <c r="E6" s="33">
+        <v>42.366700000000002</v>
+      </c>
+      <c r="F6" s="33">
+        <v>42.13</v>
+      </c>
+      <c r="G6" s="33">
+        <v>65.653999999999996</v>
+      </c>
+      <c r="H6" s="33">
+        <v>1.84E-2</v>
+      </c>
+      <c r="I6" s="33">
+        <v>0.67689999999999995</v>
+      </c>
+      <c r="J6" s="41">
+        <v>1.78E-2</v>
+      </c>
       <c r="L6" s="37"/>
       <c r="M6" s="38">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N6" s="67">
-        <f t="shared" ref="N6:S14" si="0">AVERAGE(E5,E14,E23,E32,E41)</f>
-        <v>41.142699999999998</v>
+        <f t="shared" ref="N6:S6" si="0">AVERAGE(E5,E14,E23,E32,E41)</f>
+        <v>41.128540000000001</v>
       </c>
       <c r="O6" s="67">
         <f t="shared" si="0"/>
-        <v>40.875999999999998</v>
+        <v>40.679739999999995</v>
       </c>
       <c r="P6" s="67">
         <f t="shared" si="0"/>
-        <v>50.735999999999997</v>
+        <v>50.822159999999997</v>
       </c>
       <c r="Q6" s="66">
         <f t="shared" si="0"/>
-        <v>3.3399999999999999E-2</v>
+        <v>1.9480000000000001E-2</v>
       </c>
       <c r="R6" s="66">
         <f t="shared" si="0"/>
-        <v>9.3200000000000005E-2</v>
+        <v>6.4699999999999994E-2</v>
       </c>
       <c r="S6" s="66">
         <f t="shared" si="0"/>
-        <v>1.78E-2</v>
+        <v>1.8099999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="40">
         <v>8</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="41"/>
+      <c r="D7" s="33">
+        <v>45</v>
+      </c>
+      <c r="E7" s="33">
+        <v>42.952399999999997</v>
+      </c>
+      <c r="F7" s="33">
+        <v>42.256399999999999</v>
+      </c>
+      <c r="G7" s="33">
+        <v>78.501300000000001</v>
+      </c>
+      <c r="H7" s="33">
+        <v>1.83E-2</v>
+      </c>
+      <c r="I7" s="33">
+        <v>3.6894</v>
+      </c>
+      <c r="J7" s="41">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="L7" s="40"/>
       <c r="M7" s="33">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="N7" s="67">
         <f>AVERAGE(E6,E15,E24,E33,E42)</f>
-        <v>41.8093</v>
+        <v>42.537199999999999</v>
       </c>
       <c r="O7" s="67">
-        <f t="shared" si="0"/>
-        <v>41.496699999999997</v>
+        <f t="shared" ref="O7:S14" si="1">AVERAGE(F6,F15,F24,F33,F42)</f>
+        <v>41.9724</v>
       </c>
       <c r="P7" s="67">
-        <f t="shared" si="0"/>
-        <v>65.182699999999997</v>
+        <f t="shared" si="1"/>
+        <v>66.24839999999999</v>
       </c>
       <c r="Q7" s="66">
-        <f t="shared" si="0"/>
-        <v>1.8800000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.8540000000000001E-2</v>
       </c>
       <c r="R7" s="66">
-        <f t="shared" si="0"/>
-        <v>4.0994999999999999</v>
+        <f t="shared" si="1"/>
+        <v>1.6897800000000001</v>
       </c>
       <c r="S7" s="66">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <f t="shared" si="1"/>
+        <v>1.7759999999999998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="40">
         <v>8</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="41"/>
+      <c r="D8" s="33">
+        <v>60</v>
+      </c>
+      <c r="E8" s="33">
+        <v>43.908299999999997</v>
+      </c>
+      <c r="F8" s="33">
+        <v>42.810699999999997</v>
+      </c>
+      <c r="G8" s="33">
+        <v>92.271699999999996</v>
+      </c>
+      <c r="H8" s="33">
+        <v>1.72E-2</v>
+      </c>
+      <c r="I8" s="33">
+        <v>99.524500000000003</v>
+      </c>
+      <c r="J8" s="41">
+        <v>1.6299999999999999E-2</v>
+      </c>
       <c r="L8" s="40"/>
       <c r="M8" s="33">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="N8" s="67">
-        <f t="shared" ref="N8:N14" si="1">AVERAGE(E7,E16,E25,E34,E43)</f>
-        <v>42.700400000000002</v>
+        <f t="shared" ref="N8:N14" si="2">AVERAGE(E7,E16,E25,E34,E43)</f>
+        <v>43.532959999999996</v>
       </c>
       <c r="O8" s="67">
-        <f t="shared" si="0"/>
-        <v>41.813299999999998</v>
+        <f t="shared" si="1"/>
+        <v>42.462200000000003</v>
       </c>
       <c r="P8" s="67">
-        <f t="shared" si="0"/>
-        <v>78.167100000000005</v>
+        <f t="shared" si="1"/>
+        <v>79.214480000000009</v>
       </c>
       <c r="Q8" s="66">
-        <f t="shared" si="0"/>
-        <v>1.83E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.8700000000000001E-2</v>
       </c>
       <c r="R8" s="66">
-        <f t="shared" si="0"/>
-        <v>56.718400000000003</v>
+        <f t="shared" si="1"/>
+        <v>23.586120000000001</v>
       </c>
       <c r="S8" s="66">
-        <f t="shared" si="0"/>
-        <v>1.7299999999999999E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.8180000000000002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="40">
         <v>8</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="41"/>
+      <c r="D9" s="33">
+        <v>75</v>
+      </c>
+      <c r="E9" s="33">
+        <v>44.5304</v>
+      </c>
+      <c r="F9" s="33">
+        <v>42.985100000000003</v>
+      </c>
+      <c r="G9" s="33">
+        <v>105.1845</v>
+      </c>
+      <c r="H9" s="33">
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="I9" s="33">
+        <v>1009.7265</v>
+      </c>
+      <c r="J9" s="41">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="L9" s="40"/>
       <c r="M9" s="33">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="N9" s="67">
+        <f t="shared" si="2"/>
+        <v>44.160979999999995</v>
+      </c>
+      <c r="O9" s="67">
         <f t="shared" si="1"/>
-        <v>42.766300000000001</v>
-      </c>
-      <c r="O9" s="67">
-        <f t="shared" si="0"/>
-        <v>41.708300000000001</v>
+        <v>42.770660000000007</v>
       </c>
       <c r="P9" s="67">
-        <f t="shared" si="0"/>
-        <v>90.747699999999995</v>
+        <f t="shared" si="1"/>
+        <v>92.35754</v>
       </c>
       <c r="Q9" s="66">
-        <f t="shared" si="0"/>
-        <v>1.83E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0420000000000001E-2</v>
       </c>
       <c r="R9" s="66">
-        <f t="shared" si="0"/>
-        <v>236.1413</v>
+        <f t="shared" si="1"/>
+        <v>169.29107999999999</v>
       </c>
       <c r="S9" s="66">
-        <f t="shared" si="0"/>
-        <v>1.7600000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.9019999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6454,31 +6540,31 @@
       <c r="J10" s="41"/>
       <c r="L10" s="40"/>
       <c r="M10" s="33">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="N10" s="67">
+        <f t="shared" si="2"/>
+        <v>44.633119999999998</v>
+      </c>
+      <c r="O10" s="67">
         <f t="shared" si="1"/>
-        <v>42.708300000000001</v>
-      </c>
-      <c r="O10" s="67">
-        <f t="shared" si="0"/>
-        <v>41.633099999999999</v>
+        <v>42.918080000000003</v>
       </c>
       <c r="P10" s="67">
-        <f t="shared" si="0"/>
-        <v>103.044</v>
+        <f t="shared" si="1"/>
+        <v>104.9943</v>
       </c>
       <c r="Q10" s="66">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <f t="shared" si="1"/>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="R10" s="66">
-        <f t="shared" si="0"/>
-        <v>780.51310000000001</v>
+        <f t="shared" si="1"/>
+        <v>831.17699999999991</v>
       </c>
       <c r="S10" s="66">
-        <f t="shared" si="0"/>
-        <v>1.8200000000000001E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.7299999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6493,31 +6579,29 @@
       <c r="I11" s="33"/>
       <c r="J11" s="41"/>
       <c r="L11" s="40"/>
-      <c r="M11" s="33">
-        <v>40</v>
-      </c>
+      <c r="M11" s="33"/>
       <c r="N11" s="67" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O11" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O11" s="67" t="e">
-        <f t="shared" si="0"/>
+      <c r="P11" s="67" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P11" s="67" t="e">
-        <f t="shared" si="0"/>
+      <c r="Q11" s="66" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q11" s="66" t="e">
-        <f t="shared" si="0"/>
+      <c r="R11" s="66" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R11" s="66" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="S11" s="66" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6533,31 +6617,29 @@
       <c r="I12" s="33"/>
       <c r="J12" s="41"/>
       <c r="L12" s="40"/>
-      <c r="M12" s="33">
-        <v>48</v>
-      </c>
+      <c r="M12" s="33"/>
       <c r="N12" s="67" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O12" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O12" s="67" t="e">
-        <f t="shared" si="0"/>
+      <c r="P12" s="67" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P12" s="67" t="e">
-        <f t="shared" si="0"/>
+      <c r="Q12" s="66" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q12" s="66" t="e">
-        <f t="shared" si="0"/>
+      <c r="R12" s="66" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R12" s="66" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="S12" s="66" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6573,31 +6655,29 @@
       <c r="I13" s="43"/>
       <c r="J13" s="44"/>
       <c r="L13" s="40"/>
-      <c r="M13" s="33">
-        <v>64</v>
-      </c>
+      <c r="M13" s="33"/>
       <c r="N13" s="67" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O13" s="67" t="e">
-        <f t="shared" si="0"/>
+      <c r="P13" s="67" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P13" s="67" t="e">
-        <f t="shared" si="0"/>
+      <c r="Q13" s="66" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q13" s="66" t="e">
-        <f t="shared" si="0"/>
+      <c r="R13" s="66" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R13" s="66" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="S13" s="66" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6618,24 +6698,22 @@
         <v>50.735999999999997</v>
       </c>
       <c r="H14" s="46">
-        <v>3.3399999999999999E-2</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="I14" s="46">
-        <v>9.3200000000000005E-2</v>
+        <v>8.9899999999999994E-2</v>
       </c>
       <c r="J14" s="47">
-        <v>1.78E-2</v>
+        <v>1.7899999999999999E-2</v>
       </c>
       <c r="L14" s="42"/>
-      <c r="M14" s="43">
-        <v>80</v>
-      </c>
+      <c r="M14" s="43"/>
       <c r="N14" s="67" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O14" s="67" t="e">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O14" s="67" t="e">
-        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P14" s="67" t="e">
@@ -6643,15 +6721,15 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q14" s="66" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R14" s="66" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S14" s="66" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6814,61 +6892,131 @@
       <c r="C23" s="55">
         <v>56</v>
       </c>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="57"/>
+      <c r="D23" s="56">
+        <v>15</v>
+      </c>
+      <c r="E23" s="56">
+        <v>42.031999999999996</v>
+      </c>
+      <c r="F23" s="56">
+        <v>40.58</v>
+      </c>
+      <c r="G23" s="56">
+        <v>51.122700000000002</v>
+      </c>
+      <c r="H23" s="56">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="I23" s="56">
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="J23" s="57">
+        <v>1.72E-2</v>
+      </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C24" s="55">
         <v>56</v>
       </c>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="59"/>
+      <c r="D24" s="58">
+        <v>30</v>
+      </c>
+      <c r="E24" s="58">
+        <v>43.728700000000003</v>
+      </c>
+      <c r="F24" s="58">
+        <v>42.274000000000001</v>
+      </c>
+      <c r="G24" s="58">
+        <v>66.936000000000007</v>
+      </c>
+      <c r="H24" s="58">
+        <v>1.78E-2</v>
+      </c>
+      <c r="I24" s="58">
+        <v>1.8566</v>
+      </c>
+      <c r="J24" s="59">
+        <v>1.67E-2</v>
+      </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C25" s="55">
         <v>56</v>
       </c>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="59"/>
+      <c r="D25" s="58">
+        <v>45</v>
+      </c>
+      <c r="E25" s="58">
+        <v>45.713799999999999</v>
+      </c>
+      <c r="F25" s="58">
+        <v>43.5764</v>
+      </c>
+      <c r="G25" s="58">
+        <v>81.480400000000003</v>
+      </c>
+      <c r="H25" s="58">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="I25" s="58">
+        <v>37.197699999999998</v>
+      </c>
+      <c r="J25" s="59">
+        <v>1.61E-2</v>
+      </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C26" s="55">
         <v>56</v>
       </c>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="59"/>
+      <c r="D26" s="58">
+        <v>60</v>
+      </c>
+      <c r="E26" s="58">
+        <v>46.991300000000003</v>
+      </c>
+      <c r="F26" s="58">
+        <v>44.234000000000002</v>
+      </c>
+      <c r="G26" s="58">
+        <v>95.534300000000002</v>
+      </c>
+      <c r="H26" s="58">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I26" s="58">
+        <v>247.4323</v>
+      </c>
+      <c r="J26" s="59">
+        <v>1.6500000000000001E-2</v>
+      </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C27" s="55">
         <v>56</v>
       </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="59"/>
+      <c r="D27" s="58">
+        <v>75</v>
+      </c>
+      <c r="E27" s="58">
+        <v>47.151699999999998</v>
+      </c>
+      <c r="F27" s="58">
+        <v>43.9816</v>
+      </c>
+      <c r="G27" s="58">
+        <v>107.8587</v>
+      </c>
+      <c r="H27" s="58">
+        <v>1.78E-2</v>
+      </c>
+      <c r="I27" s="58">
+        <v>991.03899999999999</v>
+      </c>
+      <c r="J27" s="59">
+        <v>1.7100000000000001E-2</v>
+      </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C28" s="55">
@@ -6918,69 +7066,139 @@
       <c r="I31" s="64"/>
       <c r="J31" s="65"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="45">
-        <v>83</v>
-      </c>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="47"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C33" s="48">
-        <v>83</v>
-      </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="49"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C34" s="48">
-        <v>83</v>
-      </c>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="49"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C35" s="48">
-        <v>83</v>
-      </c>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="49"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C36" s="48">
-        <v>83</v>
-      </c>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="49"/>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C37" s="48">
-        <v>83</v>
+        <v>990</v>
+      </c>
+      <c r="D32" s="46">
+        <v>15</v>
+      </c>
+      <c r="E32" s="46">
+        <v>40.707999999999998</v>
+      </c>
+      <c r="F32" s="46">
+        <v>40.508000000000003</v>
+      </c>
+      <c r="G32" s="46">
+        <v>51.502699999999997</v>
+      </c>
+      <c r="H32" s="46">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I32" s="46">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="J32" s="47">
+        <v>2.12E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="45">
+        <v>990</v>
+      </c>
+      <c r="D33" s="74">
+        <v>30</v>
+      </c>
+      <c r="E33" s="74">
+        <v>42.223999999999997</v>
+      </c>
+      <c r="F33" s="74">
+        <v>41.808</v>
+      </c>
+      <c r="G33" s="74">
+        <v>67.069299999999998</v>
+      </c>
+      <c r="H33" s="74">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="I33" s="74">
+        <v>1.0501</v>
+      </c>
+      <c r="J33" s="49">
+        <v>1.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="45">
+        <v>990</v>
+      </c>
+      <c r="D34" s="73">
+        <v>45</v>
+      </c>
+      <c r="E34" s="73">
+        <v>42.103999999999999</v>
+      </c>
+      <c r="F34" s="73">
+        <v>41.490200000000002</v>
+      </c>
+      <c r="G34" s="73">
+        <v>77.422700000000006</v>
+      </c>
+      <c r="H34" s="73">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="I34" s="73">
+        <v>5.4684999999999997</v>
+      </c>
+      <c r="J34" s="49">
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="45">
+        <v>990</v>
+      </c>
+      <c r="D35" s="73">
+        <v>60</v>
+      </c>
+      <c r="E35" s="73">
+        <v>42.277999999999999</v>
+      </c>
+      <c r="F35" s="73">
+        <v>41.655999999999999</v>
+      </c>
+      <c r="G35" s="73">
+        <v>89.2393</v>
+      </c>
+      <c r="H35" s="73">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="I35" s="73">
+        <v>76.664299999999997</v>
+      </c>
+      <c r="J35" s="49">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="45">
+        <v>990</v>
+      </c>
+      <c r="D36" s="72">
+        <v>75</v>
+      </c>
+      <c r="E36" s="69">
+        <v>42.678100000000001</v>
+      </c>
+      <c r="F36" s="69">
+        <v>41.847700000000003</v>
+      </c>
+      <c r="G36" s="69">
+        <v>101.17870000000001</v>
+      </c>
+      <c r="H36" s="69">
+        <v>1.9E-2</v>
+      </c>
+      <c r="I36" s="69">
+        <v>360.3082</v>
+      </c>
+      <c r="J36" s="49">
+        <v>1.7500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="45">
+        <v>990</v>
       </c>
       <c r="D37" s="69"/>
       <c r="E37" s="69"/>
@@ -6990,9 +7208,9 @@
       <c r="I37" s="69"/>
       <c r="J37" s="49"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C38" s="48">
-        <v>83</v>
+    <row r="38" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="45">
+        <v>990</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36"/>
@@ -7002,9 +7220,9 @@
       <c r="I38" s="36"/>
       <c r="J38" s="50"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C39" s="51">
-        <v>83</v>
+    <row r="39" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="45">
+        <v>990</v>
       </c>
       <c r="D39" s="69"/>
       <c r="E39" s="69"/>
@@ -7015,8 +7233,8 @@
       <c r="J39" s="49"/>
     </row>
     <row r="40" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="52">
-        <v>83</v>
+      <c r="C40" s="45">
+        <v>990</v>
       </c>
       <c r="D40" s="53"/>
       <c r="E40" s="53"/>
@@ -7030,61 +7248,1407 @@
       <c r="C41" s="55">
         <v>69</v>
       </c>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="57"/>
+      <c r="D41" s="56">
+        <v>15</v>
+      </c>
+      <c r="E41" s="56">
+        <v>41.155999999999999</v>
+      </c>
+      <c r="F41" s="56">
+        <v>40.8307</v>
+      </c>
+      <c r="G41" s="56">
+        <v>50.790700000000001</v>
+      </c>
+      <c r="H41" s="56">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I41" s="56">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="J41" s="57">
+        <v>1.6799999999999999E-2</v>
+      </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C42" s="55">
         <v>69</v>
       </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="59"/>
+      <c r="D42" s="58">
+        <v>30</v>
+      </c>
+      <c r="E42" s="58">
+        <v>42.557299999999998</v>
+      </c>
+      <c r="F42" s="58">
+        <v>42.153300000000002</v>
+      </c>
+      <c r="G42" s="58">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="H42" s="58">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="I42" s="58">
+        <v>0.76580000000000004</v>
+      </c>
+      <c r="J42" s="59">
+        <v>1.72E-2</v>
+      </c>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C43" s="55">
         <v>69</v>
       </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="59"/>
+      <c r="D43" s="58">
+        <v>45</v>
+      </c>
+      <c r="E43" s="58">
+        <v>44.194200000000002</v>
+      </c>
+      <c r="F43" s="58">
+        <v>43.174700000000001</v>
+      </c>
+      <c r="G43" s="58">
+        <v>80.500900000000001</v>
+      </c>
+      <c r="H43" s="58">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="I43" s="58">
+        <v>14.8566</v>
+      </c>
+      <c r="J43" s="59">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C44" s="55">
         <v>69</v>
       </c>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="59"/>
+      <c r="D44" s="58">
+        <v>60</v>
+      </c>
+      <c r="E44" s="58">
+        <v>44.860999999999997</v>
+      </c>
+      <c r="F44" s="58">
+        <v>43.444299999999998</v>
+      </c>
+      <c r="G44" s="58">
+        <v>93.994699999999995</v>
+      </c>
+      <c r="H44" s="58">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="I44" s="58">
+        <v>186.69300000000001</v>
+      </c>
+      <c r="J44" s="59">
+        <v>2.2700000000000001E-2</v>
+      </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C45" s="55">
         <v>69</v>
       </c>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="59"/>
+      <c r="D45" s="58">
+        <v>75</v>
+      </c>
+      <c r="E45" s="58">
+        <v>46.097099999999998</v>
+      </c>
+      <c r="F45" s="58">
+        <v>44.142899999999997</v>
+      </c>
+      <c r="G45" s="58">
+        <v>107.7056</v>
+      </c>
+      <c r="H45" s="58">
+        <v>1.78E-2</v>
+      </c>
+      <c r="I45" s="58">
+        <v>1014.2982</v>
+      </c>
+      <c r="J45" s="59">
+        <v>1.67E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C46" s="55">
+        <v>69</v>
+      </c>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="59"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C47" s="55">
+        <v>69</v>
+      </c>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="61"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C48" s="62">
+        <v>69</v>
+      </c>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="59"/>
+    </row>
+    <row r="49" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C49" s="63">
+        <v>69</v>
+      </c>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659B88F6-3D7B-4636-B90E-1B0FF835340F}">
+  <dimension ref="A1:S49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:S10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="8.88671875" style="75"/>
+    <col min="4" max="4" width="8" style="75" customWidth="1"/>
+    <col min="5" max="5" width="13" style="75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="75"/>
+    <col min="12" max="12" width="7.109375" style="75" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="75"/>
+    <col min="14" max="14" width="12" style="75" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" style="75" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" style="75" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" style="75" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" style="75" customWidth="1"/>
+    <col min="19" max="19" width="10" style="75" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="75"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+    </row>
+    <row r="4" spans="1:19" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+    </row>
+    <row r="5" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="37">
+        <v>8</v>
+      </c>
+      <c r="D5" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="38">
+        <v>50.276699999999998</v>
+      </c>
+      <c r="F5" s="38">
+        <v>49.037300000000002</v>
+      </c>
+      <c r="G5" s="38">
+        <v>76.040000000000006</v>
+      </c>
+      <c r="H5" s="38">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="I5" s="38">
+        <v>39.304099999999998</v>
+      </c>
+      <c r="J5" s="39">
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="L5" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="40">
+        <v>8</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="33">
+        <v>47.314700000000002</v>
+      </c>
+      <c r="F6" s="33">
+        <v>46.014000000000003</v>
+      </c>
+      <c r="G6" s="33">
+        <v>72.55</v>
+      </c>
+      <c r="H6" s="33">
+        <v>1.95E-2</v>
+      </c>
+      <c r="I6" s="33">
+        <v>9.1905999999999999</v>
+      </c>
+      <c r="J6" s="41">
+        <v>1.78E-2</v>
+      </c>
+      <c r="L6" s="37"/>
+      <c r="M6" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="N6" s="67">
+        <f t="shared" ref="N6:S14" si="0">AVERAGE(E5,E14,E23,E32,E41)</f>
+        <v>50.284119999999994</v>
+      </c>
+      <c r="O6" s="67">
+        <f t="shared" si="0"/>
+        <v>48.974660000000007</v>
+      </c>
+      <c r="P6" s="67">
+        <f t="shared" si="0"/>
+        <v>76.233999999999995</v>
+      </c>
+      <c r="Q6" s="66">
+        <f t="shared" si="0"/>
+        <v>1.9959999999999999E-2</v>
+      </c>
+      <c r="R6" s="66">
+        <f t="shared" si="0"/>
+        <v>32.805080000000004</v>
+      </c>
+      <c r="S6" s="66">
+        <f t="shared" si="0"/>
+        <v>1.8099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="40">
+        <v>8</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="33">
+        <v>42.366700000000002</v>
+      </c>
+      <c r="F7" s="33">
+        <v>42.13</v>
+      </c>
+      <c r="G7" s="33">
+        <v>65.653999999999996</v>
+      </c>
+      <c r="H7" s="33">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="I7" s="33">
+        <v>0.7681</v>
+      </c>
+      <c r="J7" s="41">
+        <v>1.84E-2</v>
+      </c>
+      <c r="L7" s="40"/>
+      <c r="M7" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="67">
+        <f>AVERAGE(E6,E15,E24,E33,E42)</f>
+        <v>47.344119999999997</v>
+      </c>
+      <c r="O7" s="67">
+        <f t="shared" si="0"/>
+        <v>46.154000000000011</v>
+      </c>
+      <c r="P7" s="67">
+        <f t="shared" si="0"/>
+        <v>72.901080000000007</v>
+      </c>
+      <c r="Q7" s="66">
+        <f t="shared" si="0"/>
+        <v>1.9859999999999999E-2</v>
+      </c>
+      <c r="R7" s="66">
+        <f t="shared" si="0"/>
+        <v>13.690239999999999</v>
+      </c>
+      <c r="S7" s="66">
+        <f t="shared" si="0"/>
+        <v>1.7899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="40">
+        <v>8</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="E8" s="33">
+        <v>40.978000000000002</v>
+      </c>
+      <c r="F8" s="33">
+        <v>40.171300000000002</v>
+      </c>
+      <c r="G8" s="33">
+        <v>58.798000000000002</v>
+      </c>
+      <c r="H8" s="33">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="I8" s="33">
+        <v>0.1847</v>
+      </c>
+      <c r="J8" s="41">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="L8" s="40"/>
+      <c r="M8" s="33">
+        <v>1</v>
+      </c>
+      <c r="N8" s="67">
+        <f t="shared" ref="N8:N14" si="1">AVERAGE(E7,E16,E25,E34,E43)</f>
+        <v>42.537199999999999</v>
+      </c>
+      <c r="O8" s="67">
+        <f t="shared" si="0"/>
+        <v>41.9724</v>
+      </c>
+      <c r="P8" s="67">
+        <f t="shared" si="0"/>
+        <v>66.24839999999999</v>
+      </c>
+      <c r="Q8" s="66">
+        <f t="shared" si="0"/>
+        <v>1.9339999999999996E-2</v>
+      </c>
+      <c r="R8" s="66">
+        <f t="shared" si="0"/>
+        <v>1.6475599999999999</v>
+      </c>
+      <c r="S8" s="66">
+        <f t="shared" si="0"/>
+        <v>1.8480000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="40">
+        <v>8</v>
+      </c>
+      <c r="D9" s="33">
+        <v>2</v>
+      </c>
+      <c r="E9" s="33">
+        <v>39.976700000000001</v>
+      </c>
+      <c r="F9" s="33">
+        <v>39.556699999999999</v>
+      </c>
+      <c r="G9" s="33">
+        <v>52.4893</v>
+      </c>
+      <c r="H9" s="33">
+        <v>1.83E-2</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0.21879999999999999</v>
+      </c>
+      <c r="J9" s="41">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="L9" s="40"/>
+      <c r="M9" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="N9" s="67">
+        <f t="shared" si="1"/>
+        <v>40.471879999999999</v>
+      </c>
+      <c r="O9" s="67">
+        <f t="shared" si="0"/>
+        <v>39.97092</v>
+      </c>
+      <c r="P9" s="67">
+        <f t="shared" si="0"/>
+        <v>59.624940000000002</v>
+      </c>
+      <c r="Q9" s="66">
+        <f t="shared" si="0"/>
+        <v>1.8959999999999998E-2</v>
+      </c>
+      <c r="R9" s="66">
+        <f t="shared" si="0"/>
+        <v>0.21642</v>
+      </c>
+      <c r="S9" s="66">
+        <f t="shared" si="0"/>
+        <v>1.8220000000000004E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="40">
+        <v>8</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="41"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="33">
+        <v>2</v>
+      </c>
+      <c r="N10" s="67">
+        <f t="shared" si="1"/>
+        <v>39.610300000000002</v>
+      </c>
+      <c r="O10" s="67">
+        <f t="shared" si="0"/>
+        <v>39.359480000000005</v>
+      </c>
+      <c r="P10" s="67">
+        <f t="shared" si="0"/>
+        <v>53.142920000000004</v>
+      </c>
+      <c r="Q10" s="66">
+        <f t="shared" si="0"/>
+        <v>1.9040000000000001E-2</v>
+      </c>
+      <c r="R10" s="66">
+        <f t="shared" si="0"/>
+        <v>0.14706</v>
+      </c>
+      <c r="S10" s="66">
+        <f t="shared" si="0"/>
+        <v>1.7900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="40">
+        <v>8</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="41"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="67" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O11" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q11" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R11" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S11" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="40">
+        <v>8</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="41"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="67" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O12" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q12" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R12" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S12" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="42">
+        <v>8</v>
+      </c>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="44"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="67" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O13" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P13" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q13" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R13" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S13" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="45">
+        <v>15</v>
+      </c>
+      <c r="D14" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="E14" s="46">
+        <v>49.921999999999997</v>
+      </c>
+      <c r="F14" s="46">
+        <v>48.573999999999998</v>
+      </c>
+      <c r="G14" s="46">
+        <v>75.943299999999994</v>
+      </c>
+      <c r="H14" s="46">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="I14" s="46">
+        <v>32.053800000000003</v>
+      </c>
+      <c r="J14" s="47">
+        <v>1.77E-2</v>
+      </c>
+      <c r="L14" s="42"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="67" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O14" s="67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P14" s="67" t="e">
+        <f>AVERAGE(G13,G22,G31,G40,G49)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q14" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R14" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S14" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C15" s="48">
+        <v>15</v>
+      </c>
+      <c r="D15" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="74">
+        <v>47.1233</v>
+      </c>
+      <c r="F15" s="74">
+        <v>45.718000000000004</v>
+      </c>
+      <c r="G15" s="74">
+        <v>72.355999999999995</v>
+      </c>
+      <c r="H15" s="74">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="I15" s="74">
+        <v>10.7865</v>
+      </c>
+      <c r="J15" s="49">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="Q15" s="68"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="68"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C16" s="48">
+        <v>15</v>
+      </c>
+      <c r="D16" s="74">
+        <v>1</v>
+      </c>
+      <c r="E16" s="74">
+        <v>41.8093</v>
+      </c>
+      <c r="F16" s="74">
+        <v>41.496699999999997</v>
+      </c>
+      <c r="G16" s="74">
+        <v>65.182699999999997</v>
+      </c>
+      <c r="H16" s="74">
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="I16" s="74">
+        <v>3.8742999999999999</v>
+      </c>
+      <c r="J16" s="49">
+        <v>1.83E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="48">
+        <v>15</v>
+      </c>
+      <c r="D17" s="74">
+        <v>1.5</v>
+      </c>
+      <c r="E17" s="74">
+        <v>40.323300000000003</v>
+      </c>
+      <c r="F17" s="74">
+        <v>39.859299999999998</v>
+      </c>
+      <c r="G17" s="74">
+        <v>58.046700000000001</v>
+      </c>
+      <c r="H17" s="74">
+        <v>1.9E-2</v>
+      </c>
+      <c r="I17" s="74">
+        <v>0.1724</v>
+      </c>
+      <c r="J17" s="49">
+        <v>1.7899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C18" s="48">
+        <v>15</v>
+      </c>
+      <c r="D18" s="74">
+        <v>2</v>
+      </c>
+      <c r="E18" s="74">
+        <v>39.346699999999998</v>
+      </c>
+      <c r="F18" s="74">
+        <v>39.346699999999998</v>
+      </c>
+      <c r="G18" s="74">
+        <v>51.000700000000002</v>
+      </c>
+      <c r="H18" s="74">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="I18" s="74">
+        <v>0.105</v>
+      </c>
+      <c r="J18" s="49">
+        <v>1.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C19" s="48">
+        <v>15</v>
+      </c>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="49"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C20" s="48">
+        <v>15</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="50"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C21" s="51">
+        <v>15</v>
+      </c>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="49"/>
+    </row>
+    <row r="22" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="52">
+        <v>15</v>
+      </c>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="54"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C23" s="55">
+        <v>56</v>
+      </c>
+      <c r="D23" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="56">
+        <v>50.453299999999999</v>
+      </c>
+      <c r="F23" s="56">
+        <v>49.143999999999998</v>
+      </c>
+      <c r="G23" s="56">
+        <v>76.386700000000005</v>
+      </c>
+      <c r="H23" s="56">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="I23" s="56">
+        <v>25.026700000000002</v>
+      </c>
+      <c r="J23" s="57">
+        <v>1.7600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C24" s="55">
+        <v>56</v>
+      </c>
+      <c r="D24" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="58">
+        <v>47.525300000000001</v>
+      </c>
+      <c r="F24" s="58">
+        <v>46.478000000000002</v>
+      </c>
+      <c r="G24" s="58">
+        <v>73.236699999999999</v>
+      </c>
+      <c r="H24" s="58">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="I24" s="58">
+        <v>22.592700000000001</v>
+      </c>
+      <c r="J24" s="59">
+        <v>1.7899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C25" s="55">
+        <v>56</v>
+      </c>
+      <c r="D25" s="58">
+        <v>1</v>
+      </c>
+      <c r="E25" s="58">
+        <v>43.728700000000003</v>
+      </c>
+      <c r="F25" s="58">
+        <v>42.274000000000001</v>
+      </c>
+      <c r="G25" s="58">
+        <v>66.936000000000007</v>
+      </c>
+      <c r="H25" s="58">
+        <v>1.9199999999999998E-2</v>
+      </c>
+      <c r="I25" s="58">
+        <v>1.8932</v>
+      </c>
+      <c r="J25" s="59">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="55">
+        <v>56</v>
+      </c>
+      <c r="D26" s="58">
+        <v>1.5</v>
+      </c>
+      <c r="E26" s="58">
+        <v>39.936700000000002</v>
+      </c>
+      <c r="F26" s="58">
+        <v>39.8093</v>
+      </c>
+      <c r="G26" s="58">
+        <v>60.56</v>
+      </c>
+      <c r="H26" s="58">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="I26" s="58">
+        <v>0.2258</v>
+      </c>
+      <c r="J26" s="59">
+        <v>1.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C27" s="55">
+        <v>56</v>
+      </c>
+      <c r="D27" s="58">
+        <v>2</v>
+      </c>
+      <c r="E27" s="58">
+        <v>39.372700000000002</v>
+      </c>
+      <c r="F27" s="58">
+        <v>39.212699999999998</v>
+      </c>
+      <c r="G27" s="58">
+        <v>54.323300000000003</v>
+      </c>
+      <c r="H27" s="58">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="I27" s="58">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="J27" s="59">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C28" s="55">
+        <v>56</v>
+      </c>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="59"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C29" s="55">
+        <v>56</v>
+      </c>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="61"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C30" s="62">
+        <v>56</v>
+      </c>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="59"/>
+    </row>
+    <row r="31" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="63">
+        <v>56</v>
+      </c>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="65"/>
+    </row>
+    <row r="32" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="45">
+        <v>990</v>
+      </c>
+      <c r="D32" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="E32" s="46">
+        <v>50.385300000000001</v>
+      </c>
+      <c r="F32" s="46">
+        <v>49.043999999999997</v>
+      </c>
+      <c r="G32" s="46">
+        <v>76.4833</v>
+      </c>
+      <c r="H32" s="46">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="I32" s="46">
+        <v>43.949800000000003</v>
+      </c>
+      <c r="J32" s="47">
+        <v>1.7600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="45">
+        <v>990</v>
+      </c>
+      <c r="D33" s="74">
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="74">
+        <v>47.518000000000001</v>
+      </c>
+      <c r="F33" s="74">
+        <v>46.329300000000003</v>
+      </c>
+      <c r="G33" s="74">
+        <v>73.346000000000004</v>
+      </c>
+      <c r="H33" s="74">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="I33" s="74">
+        <v>14.815200000000001</v>
+      </c>
+      <c r="J33" s="49">
+        <v>1.77E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="45">
+        <v>990</v>
+      </c>
+      <c r="D34" s="74">
+        <v>1</v>
+      </c>
+      <c r="E34" s="74">
+        <v>42.223999999999997</v>
+      </c>
+      <c r="F34" s="74">
+        <v>41.808</v>
+      </c>
+      <c r="G34" s="74">
+        <v>67.069299999999998</v>
+      </c>
+      <c r="H34" s="74">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="I34" s="74">
+        <v>1.0391999999999999</v>
+      </c>
+      <c r="J34" s="49">
+        <v>1.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="45">
+        <v>990</v>
+      </c>
+      <c r="D35" s="74">
+        <v>1.5</v>
+      </c>
+      <c r="E35" s="74">
+        <v>39.720700000000001</v>
+      </c>
+      <c r="F35" s="74">
+        <v>39.631999999999998</v>
+      </c>
+      <c r="G35" s="74">
+        <v>60.84</v>
+      </c>
+      <c r="H35" s="74">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="I35" s="74">
+        <v>0.1905</v>
+      </c>
+      <c r="J35" s="49">
+        <v>1.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="45">
+        <v>990</v>
+      </c>
+      <c r="D36" s="74">
+        <v>2</v>
+      </c>
+      <c r="E36" s="74">
+        <v>39.756700000000002</v>
+      </c>
+      <c r="F36" s="74">
+        <v>39.197299999999998</v>
+      </c>
+      <c r="G36" s="74">
+        <v>54.627299999999998</v>
+      </c>
+      <c r="H36" s="74">
+        <v>1.95E-2</v>
+      </c>
+      <c r="I36" s="74">
+        <v>0.15909999999999999</v>
+      </c>
+      <c r="J36" s="49">
+        <v>1.7600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="45">
+        <v>990</v>
+      </c>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="49"/>
+    </row>
+    <row r="38" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="45">
+        <v>990</v>
+      </c>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="50"/>
+    </row>
+    <row r="39" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="45">
+        <v>990</v>
+      </c>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="49"/>
+    </row>
+    <row r="40" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="45">
+        <v>990</v>
+      </c>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="54"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C41" s="55">
+        <v>69</v>
+      </c>
+      <c r="D41" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="E41" s="56">
+        <v>50.383299999999998</v>
+      </c>
+      <c r="F41" s="56">
+        <v>49.073999999999998</v>
+      </c>
+      <c r="G41" s="56">
+        <v>76.316699999999997</v>
+      </c>
+      <c r="H41" s="56">
+        <v>1.95E-2</v>
+      </c>
+      <c r="I41" s="56">
+        <v>23.690999999999999</v>
+      </c>
+      <c r="J41" s="57">
+        <v>1.8200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C42" s="55">
+        <v>69</v>
+      </c>
+      <c r="D42" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="58">
+        <v>47.2393</v>
+      </c>
+      <c r="F42" s="58">
+        <v>46.230699999999999</v>
+      </c>
+      <c r="G42" s="58">
+        <v>73.0167</v>
+      </c>
+      <c r="H42" s="58">
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="I42" s="58">
+        <v>11.0662</v>
+      </c>
+      <c r="J42" s="59">
+        <v>1.7600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C43" s="55">
+        <v>69</v>
+      </c>
+      <c r="D43" s="58">
+        <v>1</v>
+      </c>
+      <c r="E43" s="58">
+        <v>42.557299999999998</v>
+      </c>
+      <c r="F43" s="58">
+        <v>42.153300000000002</v>
+      </c>
+      <c r="G43" s="58">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="H43" s="58">
+        <v>1.9199999999999998E-2</v>
+      </c>
+      <c r="I43" s="58">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="J43" s="59">
+        <v>1.7600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C44" s="55">
+        <v>69</v>
+      </c>
+      <c r="D44" s="58">
+        <v>1.5</v>
+      </c>
+      <c r="E44" s="58">
+        <v>41.400700000000001</v>
+      </c>
+      <c r="F44" s="58">
+        <v>40.3827</v>
+      </c>
+      <c r="G44" s="58">
+        <v>59.88</v>
+      </c>
+      <c r="H44" s="58">
+        <v>1.89E-2</v>
+      </c>
+      <c r="I44" s="58">
+        <v>0.30869999999999997</v>
+      </c>
+      <c r="J44" s="59">
+        <v>1.8499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C45" s="55">
+        <v>69</v>
+      </c>
+      <c r="D45" s="58">
+        <v>2</v>
+      </c>
+      <c r="E45" s="58">
+        <v>39.598700000000001</v>
+      </c>
+      <c r="F45" s="58">
+        <v>39.484000000000002</v>
+      </c>
+      <c r="G45" s="58">
+        <v>53.274000000000001</v>
+      </c>
+      <c r="H45" s="58">
+        <v>1.89E-2</v>
+      </c>
+      <c r="I45" s="58">
+        <v>0.13339999999999999</v>
+      </c>
+      <c r="J45" s="59">
+        <v>1.7899999999999999E-2</v>
+      </c>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C46" s="55">

</xml_diff>